<commit_message>
Updated ExperimentDescription with results, and added some more notes to results sheet
</commit_message>
<xml_diff>
--- a/results/results_02-26-18-34.xlsx
+++ b/results/results_02-26-18-34.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oxeye\CMP220-Git\java-collection-performance-JeffreyCoxChatham\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DAD49A4-E026-4D7A-AD29-E815747B72B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF59B9C6-8338-4A90-8953-CB233B4A0BC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="19416" xr2:uid="{DC66C24C-3254-4EA2-ACBC-81561BA45FA4}"/>
+    <workbookView xWindow="528" yWindow="3444" windowWidth="23040" windowHeight="14100" xr2:uid="{DC66C24C-3254-4EA2-ACBC-81561BA45FA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>Array</t>
   </si>
@@ -56,7 +56,13 @@
     <t>Write</t>
   </si>
   <si>
-    <t>Note: For the Vector Write Test, the 1-minute cap was disabled, as it seemed likely it would still finish within ~100 seconds, and its value was still reasonable to be recorded. The Read and Write Test times for Linked Lists, for comparison, were getting absurd.</t>
+    <t>Note 2: values of 0.000 were entered as 0.0005, so that they could still be graphed on the log10 scale. Tests above 60 real-time seconds were aborted automatically by the failsafe.</t>
+  </si>
+  <si>
+    <t>Note 3: For the Vector Write Test, the 1-minute cap was disabled, as it seemed likely it would still finish within ~100 seconds, and its value was still reasonable to be recorded. The Read and Write Test times for Linked Lists, for comparison, were getting absurd.</t>
+  </si>
+  <si>
+    <t>Note 1: For the linked list read and write tests, times were heavily approximated. See ExperimentDescription.txt for details.</t>
   </si>
 </sst>
 </file>
@@ -3340,15 +3346,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
+      <xdr:colOff>365760</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3376,15 +3382,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
+      <xdr:colOff>388620</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3412,15 +3418,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>601980</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>297180</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3765,10 +3771,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8800941-9362-40A7-8AF3-564FF0C53939}">
-  <dimension ref="A1:N41"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3991,9 +3997,19 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>